<commit_message>
Terminado o arquivo .plist
Arquivo contendo todos os lugares escolhidos e lat/long
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32220" yWindow="2480" windowWidth="19000" windowHeight="27540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2475" windowWidth="9690" windowHeight="1815" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Endereço</t>
   </si>
@@ -255,12 +255,50 @@
   <si>
     <t>Avenida Paulista, 2073 – Jardim Paulista – São Paulo</t>
   </si>
+  <si>
+    <t>Concreto # Cultura Urbana e Contracultura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arte urbana e contracultura são as principais diretrizes do mais novo centro de cultura paulistano, inaugurado em novembro de 2010, com a proposta de incentivar, democratizar e mostrar as diferentes formas de expressão que afloram na cidade grande. </t>
+  </si>
+  <si>
+    <t>Rua Fradique Coutinho, 1209 – Vila Madalena</t>
+  </si>
+  <si>
+    <t>Edificio Itália</t>
+  </si>
+  <si>
+    <t>Construído em 1956, o Edifício Itália foi por muito tempo o maior edifício da cidade de São Paulo, com 165 metros (hoje, é o segundo maior) e é um dos pontos turísticos mais visitados da capital, devido à vista 360º da cidade que seu terraço, onde se localiza o restaurante Terraço Itália, proporciona.
+Ocupado em sua maior parte por escritórios, o edifício abriga também, em seus três primeiros andares, a associação Circolo Italiano, nome oficial do edifício.</t>
+  </si>
+  <si>
+    <t>Avenida Ipiranga, 344  – República – Centro</t>
+  </si>
+  <si>
+    <t>Edificio Martineli</t>
+  </si>
+  <si>
+    <t>Rua São Bento, 500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O primeiro arranha céu da América Latina, o Edifício Martinelli está localizado no centro de São Paulo entre as ruas São Bento, Av. São João e a Rua Libero Badaró 
+O Edifício foi projetado pelo seu idealizador, o italiano Giuseppe Martinelli, em 1924 e simbolizou progresso da cidade. Mais de 600 operários trabalharam nas obras. A construção foi iniciada em 1924 e a inauguração aconteceu em 1929, com 20 andares. </t>
+  </si>
+  <si>
+    <t>Estação da Luz</t>
+  </si>
+  <si>
+    <t>Praça da Luz, 1 - Luz </t>
+  </si>
+  <si>
+    <t>Aberta ao público em 1º de março de 1901, a Estação da Luz ocupa 7,5 mil m² do Jardim da Luz, onde se encontram as estruturas trazidas da Inglaterra que copiam o Big Ben e a abadia de Westminter. Não houve inauguração, já que o tráfego foi sendo deslocado aos poucos, mas não demorou muito para que o novo marco da cidade fosse considerado uma sala de visitas de São Paulo. Todas as personalidades ilustres que tinham a capital como destino eram obrigadas a desembarcar no local. Empresários, intelectuais, políticos, diplomatas e reis foram recepcionados em seu saguão e por lá passavam ao se despedirem.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -310,6 +348,24 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -350,7 +406,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,31 +421,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="20">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -715,24 +779,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="46.375" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -755,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -778,7 +842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -801,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -824,7 +888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17">
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -847,7 +911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17">
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -870,7 +934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17">
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -893,7 +957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17">
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -916,7 +980,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17">
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -939,7 +1003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17">
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -962,7 +1026,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -985,7 +1049,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17">
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1008,7 +1072,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17">
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1031,7 +1095,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17">
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1054,7 +1118,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17">
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1077,7 +1141,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17" customHeight="1">
+    <row r="17" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1100,7 +1164,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" customHeight="1">
+    <row r="18" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1123,7 +1187,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17">
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1146,7 +1210,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17">
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1169,7 +1233,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17">
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1192,7 +1256,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17">
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1213,6 +1277,92 @@
       </c>
       <c r="G22" s="2" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="10">
+        <v>-23556943</v>
+      </c>
+      <c r="F23" s="10">
+        <v>-46690783</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="10">
+        <v>-23545360</v>
+      </c>
+      <c r="F24" s="10">
+        <v>-46643844</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="10">
+        <v>-23545466</v>
+      </c>
+      <c r="F25" s="10">
+        <v>-46634914</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1220,7 +1370,7 @@
     <hyperlink ref="G9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>